<commit_message>
Adding stl's and updated xlsx
</commit_message>
<xml_diff>
--- a/Heated Bed/Heated Bed Power Calcs.xlsx
+++ b/Heated Bed/Heated Bed Power Calcs.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darren.pruitt\Dropbox\Maker\3D Print\Rostock Max\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darren.pruitt\Dropbox\Maker\3D Print\Github\RostockMaxV2_Duet\Heated Bed\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1608" yWindow="132" windowWidth="25872" windowHeight="13092"/>
+    <workbookView xWindow="2736" yWindow="132" windowWidth="25872" windowHeight="13092"/>
   </bookViews>
   <sheets>
     <sheet name="VIR" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -48,8 +48,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -62,8 +70,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -71,19 +84,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1"/>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -101,18 +147,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E5" totalsRowShown="0">
-  <autoFilter ref="A1:E5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E6" totalsRowShown="0">
+  <autoFilter ref="A1:E6"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Volt"/>
     <tableColumn id="2" name="Resistance (ohms)"/>
-    <tableColumn id="3" name="Current (amp)">
+    <tableColumn id="3" name="Current (amp)" dataCellStyle="Normal">
       <calculatedColumnFormula>Table1[Volt]/Table1[Resistance (ohms)]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="Power (Watt)">
       <calculatedColumnFormula>Table1[Volt]*Table1[Current (amp)]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Max Bed Power" dataDxfId="0">
+    <tableColumn id="5" name="Max Bed Power" dataDxfId="2">
       <calculatedColumnFormula>255*Table1[[#This Row],[Power (Watt)]]/D1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -196,6 +242,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -231,6 +294,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -407,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,7 +529,7 @@
         <f>Table1[Volt]/Table1[Resistance (ohms)]</f>
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <f>Table1[Volt]*Table1[Current (amp)]</f>
         <v>120</v>
       </c>
@@ -468,7 +548,7 @@
         <f>Table1[Volt]/Table1[Resistance (ohms)]</f>
         <v>20</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <f>Table1[Volt]*Table1[Current (amp)]</f>
         <v>480</v>
       </c>
@@ -477,7 +557,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="3">
         <f>Table1[[#This Row],[Resistance (ohms)]]*Table1[[#This Row],[Current (amp)]]</f>
         <v>18</v>
       </c>
@@ -487,7 +567,7 @@
       <c r="C4">
         <v>15</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <f>Table1[Volt]*Table1[Current (amp)]</f>
         <v>270</v>
       </c>
@@ -497,7 +577,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="A5" s="4">
         <f>(Table1[[#This Row],[Power (Watt)]]*Table1[[#This Row],[Resistance (ohms)]])^0.5</f>
         <v>16.970562748477139</v>
       </c>
@@ -507,7 +587,7 @@
       <c r="C5">
         <v>15</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <f>D3/2</f>
         <v>240</v>
       </c>
@@ -516,7 +596,32 @@
         <v>127.5</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>1.2</v>
+      </c>
+      <c r="C6" s="1">
+        <f>Table1[Volt]/Table1[Resistance (ohms)]</f>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="D6" s="4">
+        <f>Table1[Volt]*Table1[Current (amp)]</f>
+        <v>333.33333333333337</v>
+      </c>
+      <c r="E6" s="1">
+        <f>MIN(255, 255*Table1[[#This Row],[Power (Watt)]]/D5)</f>
+        <v>255</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:C6">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$C$2&gt;15</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>